<commit_message>
Test Create Account Component
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emad\Desktop\maidsTask\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MyWork\RPA Project\MaidsProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB81AABC-2427-4A88-B7CC-A4449BDA5FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F8DDA5-3000-454A-AC01-55AA2E6FC9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>hidemeUsername</t>
   </si>
   <si>
-    <t>rpaTest253272</t>
-  </si>
-  <si>
     <t>username of hide.me account to signup or login</t>
   </si>
   <si>
@@ -174,13 +171,16 @@
   </si>
   <si>
     <t xml:space="preserve">FROM </t>
+  </si>
+  <si>
+    <t>emadRageb123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -195,13 +195,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -242,11 +235,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -255,25 +247,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,7 +483,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -516,22 +506,22 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>20</v>
+      <c r="B2" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -542,217 +532,212 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>45</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="B11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>23</v>
+      <c r="A12" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B12" s="3">
         <v>993</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="7" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="7" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="6">
+        <v>50</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="7">
-        <v>50</v>
-      </c>
-      <c r="C15" s="7" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="6">
+        <v>15000</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="6">
+        <v>30000</v>
+      </c>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="7">
-        <v>15000</v>
-      </c>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="7">
-        <v>30000</v>
-      </c>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>3</v>
       </c>
-      <c r="C21" s="7"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>19</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{AC209DB5-A2AE-4E79-986D-D962D56F0D89}"/>
-    <hyperlink ref="B19" r:id="rId2" xr:uid="{34BA0630-96AB-4DB5-8026-A67086AB4A6B}"/>
-    <hyperlink ref="B11" r:id="rId3" xr:uid="{20A3029F-B384-427A-86AE-21C63B25B919}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
End Logout Component And Tested
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MyWork\RPA Project\MaidsProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F8DDA5-3000-454A-AC01-55AA2E6FC9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958BE131-5066-436D-B4C7-D6BC85426C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,7 +261,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,7 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -604,7 +604,7 @@
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="4"/>
@@ -686,7 +686,7 @@
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="6"/>

</xml_diff>

<commit_message>
End Create Account And Log in And out Process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MyWork\RPA Project\MaidsProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958BE131-5066-436D-B4C7-D6BC85426C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4931BA65-7416-4C14-9EDA-30EE1A53F6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,9 +155,6 @@
     <t>mailFilterTypeSubject</t>
   </si>
   <si>
-    <t>SUBJECT</t>
-  </si>
-  <si>
     <t>mailFIlterSubjectValue</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>emadRageb123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBJECT </t>
   </si>
 </sst>
 </file>
@@ -238,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -261,7 +261,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +482,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -509,7 +508,7 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -532,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -576,13 +575,13 @@
         <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>21</v>
@@ -593,19 +592,19 @@
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4"/>
     </row>

</xml_diff>

<commit_message>
End Hide Me Account But Need Some Refactor
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MyWork\RPA Project\MaidsProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4931BA65-7416-4C14-9EDA-30EE1A53F6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E07DD04-5D82-42E4-8E28-3D9D41C3F7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,13 +482,13 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="12.6640625" style="3"/>
   </cols>

</xml_diff>